<commit_message>
Agenda: nÃ£o pedir config enquanto carrega do banco; CRUD usuÃ¡rios e permissÃµes; Obras CRUD, modal e API; ajustes de UI e design
</commit_message>
<xml_diff>
--- a/geralobras.xlsx
+++ b/geralobras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robso\OneDrive\Documentos\Coorporativo\copilot 2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213B52F1-559C-4689-80CD-FA0F82CDC3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E55C8D-CFB6-477A-B6FB-ECC1F10C67F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="9" xr2:uid="{85042D99-AF67-46D0-BBD8-7613075613E7}"/>
   </bookViews>
@@ -5361,7 +5361,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>